<commit_message>
Added Full Backtester 1
</commit_message>
<xml_diff>
--- a/BackTesterConfig.xlsx
+++ b/BackTesterConfig.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicholastorres/Coding/HAVEN-MK-3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F86F8937-5C28-9E48-AC19-763C042BE9C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABF88F98-CB1D-EA4B-AE1B-298BD46035B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="14700" windowHeight="18360" xr2:uid="{4C302A0A-2DAA-6D4A-B671-BE37219EA0D1}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="17">
   <si>
     <t>Parameter</t>
   </si>
@@ -47,43 +47,46 @@
     <t>Enabled</t>
   </si>
   <si>
-    <t>3 Month Growth</t>
-  </si>
-  <si>
-    <t>minimum</t>
-  </si>
-  <si>
-    <t>maximum</t>
-  </si>
-  <si>
     <t>Subparameter</t>
   </si>
   <si>
-    <t>sma</t>
-  </si>
-  <si>
-    <t>short</t>
-  </si>
-  <si>
-    <t>long</t>
-  </si>
-  <si>
     <t>Default</t>
   </si>
   <si>
-    <t>ema</t>
-  </si>
-  <si>
     <t>rsi</t>
   </si>
   <si>
-    <t>Description</t>
-  </si>
-  <si>
     <t>length</t>
   </si>
   <si>
-    <t>adx</t>
+    <t>stoch</t>
+  </si>
+  <si>
+    <t>k</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>klen</t>
+  </si>
+  <si>
+    <t>sma10</t>
+  </si>
+  <si>
+    <t>atrts</t>
+  </si>
+  <si>
+    <t>growth</t>
+  </si>
+  <si>
+    <t>oneyear</t>
+  </si>
+  <si>
+    <t>threemonths</t>
+  </si>
+  <si>
+    <t>atr</t>
   </si>
 </sst>
 </file>
@@ -125,9 +128,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -464,10 +470,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E80EB44A-54EA-4E49-BAFB-5459F2DCBDE8}">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="F11" activeCellId="1" sqref="E3 F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -477,12 +483,12 @@
     <col min="3" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -491,134 +497,142 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="1">
         <v>10</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="1">
-        <v>10</v>
-      </c>
-      <c r="D2" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="E2" s="1">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="1">
-        <v>50</v>
-      </c>
-      <c r="D3" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="E3" s="1">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="1">
-        <v>20</v>
-      </c>
       <c r="D4" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="E4" s="1">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="1">
+        <v>14</v>
+      </c>
+      <c r="D5" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="1">
-        <v>50</v>
-      </c>
-      <c r="D5" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="E5" s="1">
+      <c r="C6" s="1">
+        <v>3</v>
+      </c>
+      <c r="D6" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="1" t="s">
+      <c r="C7" s="1">
+        <v>3</v>
+      </c>
+      <c r="D7" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="1">
+        <v>14</v>
+      </c>
+      <c r="D8" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="E6" s="1">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="E7" s="1">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
+      <c r="C9" s="1">
+        <v>3</v>
+      </c>
+      <c r="D9" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="1">
         <v>14</v>
       </c>
-      <c r="D8" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="E8" s="1">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9" s="1" t="s">
+      <c r="D10" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="1">
         <v>14</v>
       </c>
-      <c r="D9" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="E9" s="1">
-        <v>10</v>
+      <c r="D11" s="1" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>